<commit_message>
Models and figures finalized
</commit_message>
<xml_diff>
--- a/sapling_oct_2020.xlsx
+++ b/sapling_oct_2020.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20398"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20399"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ty00osat\Documents\PhD\Grass-fire experiment\Analysis\sapling_eghats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46AC4C91-A237-4D49-B44E-51EB76C26508}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F449AC89-1504-49BB-9662-763B754CFC37}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7070" xr2:uid="{1CE48C09-7398-BC45-9608-28956C5ABA37}"/>
   </bookViews>
@@ -23,7 +23,7 @@
   <calcPr calcId="191029"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId4"/>
-    <pivotCache cacheId="5" r:id="rId5"/>
+    <pivotCache cacheId="1" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -23902,7 +23902,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C60DD2B7-DDBA-4669-AA8E-81120085A1BD}" name="PivotTable2" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C60DD2B7-DDBA-4669-AA8E-81120085A1BD}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
   <location ref="A3:E8" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField showAll="0"/>
@@ -24332,8 +24332,8 @@
   <dimension ref="A1:I995"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+      <pane ySplit="1" topLeftCell="A127" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E596" sqref="E596"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -24605,7 +24605,7 @@
         <v>1.9</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>136</v>
@@ -25901,7 +25901,7 @@
         <v>1044</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F54" s="1">
         <v>18</v>
@@ -26220,7 +26220,7 @@
         <v>1051</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F65" s="1">
         <v>19</v>
@@ -26887,7 +26887,7 @@
         <v>1069</v>
       </c>
       <c r="E88" s="4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="F88" s="1">
         <v>115</v>
@@ -27061,7 +27061,7 @@
         <v>1073</v>
       </c>
       <c r="E94" s="4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F94" s="1">
         <v>31</v>
@@ -32203,7 +32203,7 @@
         <v>2.6</v>
       </c>
       <c r="H271" s="4" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="I271" s="10" t="s">
         <v>136</v>
@@ -34891,7 +34891,7 @@
         <v>1444</v>
       </c>
       <c r="E364" s="4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="F364" s="1">
         <v>93</v>
@@ -36428,7 +36428,7 @@
         <v>3403</v>
       </c>
       <c r="E417" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F417" s="1">
         <v>98</v>
@@ -36756,7 +36756,7 @@
         <v>1.9</v>
       </c>
       <c r="H428" s="4" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="I428" s="10" t="s">
         <v>136</v>
@@ -39424,7 +39424,7 @@
         <v>2.4</v>
       </c>
       <c r="H520" s="4" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="I520" s="10" t="s">
         <v>140</v>
@@ -39482,7 +39482,7 @@
         <v>2</v>
       </c>
       <c r="H522" s="4" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="I522" s="10" t="s">
         <v>140</v>
@@ -39801,7 +39801,7 @@
         <v>1.3</v>
       </c>
       <c r="H533" s="4" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="I533" s="10" t="s">
         <v>140</v>
@@ -40323,7 +40323,7 @@
         <v>3.2</v>
       </c>
       <c r="H551" s="4" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="I551" s="10" t="s">
         <v>140</v>
@@ -41590,7 +41590,7 @@
         <v>3901</v>
       </c>
       <c r="E595" s="4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F595" s="1">
         <v>115</v>
@@ -44238,7 +44238,7 @@
         <v>3.8</v>
       </c>
       <c r="H686" s="4" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="I686" s="10" t="s">
         <v>140</v>

</xml_diff>